<commit_message>
refactoring: extracted working with excel methods
</commit_message>
<xml_diff>
--- a/datasheet.xlsx
+++ b/datasheet.xlsx
@@ -80,14 +80,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,21 +399,21 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -421,7 +421,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -429,7 +429,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">

</xml_diff>